<commit_message>
create_tazdata_devpipeline_map.py - fix aggfunc in pivot to sum
And also add activity/human readable labels to pipeline
</commit_message>
<xml_diff>
--- a/TableauAliases.xlsx
+++ b/TableauAliases.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\petrale\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDC8E46C-66D4-40B6-80C2-600DF4DA640A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2975956-17A7-4E7B-97B8-7455ABE64B48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2085" yWindow="3645" windowWidth="29040" windowHeight="15510" xr2:uid="{F81C04E2-57B8-4074-942F-B8B7442EF60A}"/>
+    <workbookView xWindow="19890" yWindow="5550" windowWidth="18120" windowHeight="13485" xr2:uid="{F81C04E2-57B8-4074-942F-B8B7442EF60A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="building_type" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="77">
   <si>
     <t>building_type_descr</t>
   </si>
@@ -234,26 +234,109 @@
   </si>
   <si>
     <t>???</t>
+  </si>
+  <si>
+    <t>Activity</t>
+  </si>
+  <si>
+    <t>3000 Industrial, manufacturing, and waste-related</t>
+  </si>
+  <si>
+    <t>5000 Travel or movement activities</t>
+  </si>
+  <si>
+    <t>1000 Residential activities (SF)</t>
+  </si>
+  <si>
+    <t>1000 Residential activities (MF)</t>
+  </si>
+  <si>
+    <t>2000 Shopping, business, or trade activities</t>
+  </si>
+  <si>
+    <t>4000 Social, institutional, or infrastructure related activities</t>
+  </si>
+  <si>
+    <t>1500 Mixed use activities</t>
+  </si>
+  <si>
+    <t>9000 No human activity or unclassifiable activity</t>
+  </si>
+  <si>
+    <t>7000 Leisure activities</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF996633"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -268,14 +351,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF996633"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -584,21 +684,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{245EA375-1D2B-450F-BC78-A546918D06FC}">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
     <col min="2" max="2" width="33" customWidth="1"/>
-    <col min="4" max="4" width="35.5703125" customWidth="1"/>
+    <col min="3" max="3" width="44.7109375" customWidth="1"/>
+    <col min="4" max="4" width="54.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -608,200 +709,251 @@
       <c r="C1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="C2" t="str">
         <f>_xlfn.CONCAT(A2," - ",B2)</f>
+        <v>AL - assisted living</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" t="str">
+        <f>_xlfn.CONCAT(A3," - ",B3)</f>
+        <v>CM - condo or apt common area</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="str">
+        <f>_xlfn.CONCAT(A4," - ",B4)</f>
+        <v>DM - dorm or shelter</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="str">
+        <f>_xlfn.CONCAT(A5," - ",B5)</f>
+        <v>SR - single room occupancy</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="str">
+        <f>_xlfn.CONCAT(A6," - ",B6)</f>
+        <v>HM - multi family residential</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" t="str">
+        <f>_xlfn.CONCAT(A7," - ",B7)</f>
         <v>HS - single family residential</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="D7" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B8" t="s">
         <v>21</v>
       </c>
-      <c r="C3" t="str">
-        <f t="shared" ref="C3:C33" si="0">_xlfn.CONCAT(A3," - ",B3)</f>
+      <c r="C8" t="str">
+        <f>_xlfn.CONCAT(A8," - ",B8)</f>
         <v>HT - townhomes</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" t="str">
-        <f t="shared" si="0"/>
-        <v>HM - multi family residential</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="D8" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>34</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B9" t="s">
         <v>23</v>
       </c>
-      <c r="C5" t="str">
-        <f t="shared" si="0"/>
+      <c r="C9" t="str">
+        <f>_xlfn.CONCAT(A9," - ",B9)</f>
         <v>MH - mobile home</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" t="str">
-        <f t="shared" si="0"/>
-        <v>SR - single room occupancy</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" t="str">
-        <f t="shared" si="0"/>
-        <v>AL - assisted living</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" t="str">
-        <f t="shared" si="0"/>
-        <v>DM - dorm or shelter</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" t="str">
-        <f t="shared" si="0"/>
-        <v>CM - condo or apt common area</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" t="str">
+        <f>_xlfn.CONCAT(A10," - ",B10)</f>
+        <v>ME - mixed use employment focused</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" t="str">
+        <f>_xlfn.CONCAT(A11," - ",B11)</f>
+        <v>MR - mixed use residential focused</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" t="str">
+        <f>_xlfn.CONCAT(A12," - ",B12)</f>
+        <v>MT - mixed use industrial focused</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" t="str">
+        <f>_xlfn.CONCAT(A13," - ",B13)</f>
+        <v>HO - hotel</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>7</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B14" t="s">
         <v>28</v>
       </c>
-      <c r="C10" t="str">
-        <f t="shared" si="0"/>
+      <c r="C14" t="str">
+        <f>_xlfn.CONCAT(A14," - ",B14)</f>
         <v>OF - office</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B11" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" t="str">
-        <f t="shared" si="0"/>
-        <v>GV - gov</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" t="s">
-        <v>66</v>
-      </c>
-      <c r="C12" t="str">
-        <f t="shared" si="0"/>
-        <v>GQ - ???</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" t="str">
-        <f t="shared" si="0"/>
-        <v>HP - hospital</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" t="str">
-        <f t="shared" si="0"/>
-        <v>HO - hotel</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D14" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="C15" t="str">
-        <f t="shared" si="0"/>
-        <v>SC - k12 school</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+        <f>_xlfn.CONCAT(A15," - ",B15)</f>
+        <v>RB - retail big box or regional</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B16" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="C16" t="str">
-        <f t="shared" si="0"/>
-        <v>UN - college or university</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+        <f>_xlfn.CONCAT(A16," - ",B16)</f>
+        <v>RF - retail food or drink</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C17" t="str">
-        <f t="shared" si="0"/>
-        <v>IL - light industrial</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+        <f>_xlfn.CONCAT(A17," - ",B17)</f>
+        <v>RS - retail general</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>42</v>
       </c>
@@ -809,191 +961,244 @@
         <v>49</v>
       </c>
       <c r="C18" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(A18," - ",B18)</f>
         <v>FP - food processing and wineries</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D18" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" t="str">
+        <f>_xlfn.CONCAT(A19," - ",B19)</f>
+        <v>IH - heavy industrial</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" t="str">
+        <f>_xlfn.CONCAT(A20," - ",B20)</f>
+        <v>IL - light industrial</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>11</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B21" t="s">
         <v>50</v>
       </c>
-      <c r="C19" t="str">
-        <f t="shared" si="0"/>
+      <c r="C21" t="str">
+        <f>_xlfn.CONCAT(A21," - ",B21)</f>
         <v>IW - warehouse or logistics</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>12</v>
-      </c>
-      <c r="B20" t="s">
-        <v>51</v>
-      </c>
-      <c r="C20" t="str">
-        <f t="shared" si="0"/>
-        <v>IH - heavy industrial</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" t="s">
-        <v>52</v>
-      </c>
-      <c r="C21" t="str">
-        <f t="shared" si="0"/>
-        <v>RS - retail general</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D21" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B22" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="C22" t="str">
-        <f t="shared" si="0"/>
-        <v>RB - retail big box or regional</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+        <f>_xlfn.CONCAT(A22," - ",B22)</f>
+        <v>GQ - ???</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="B23" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="C23" t="str">
-        <f t="shared" si="0"/>
-        <v>MR - mixed use residential focused</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+        <f>_xlfn.CONCAT(A23," - ",B23)</f>
+        <v>GV - gov</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="B24" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="C24" t="str">
-        <f t="shared" si="0"/>
-        <v>MT - mixed use industrial focused</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+        <f>_xlfn.CONCAT(A24," - ",B24)</f>
+        <v>HP - hospital</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="B25" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="C25" t="str">
-        <f t="shared" si="0"/>
-        <v>ME - mixed use employment focused</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+        <f>_xlfn.CONCAT(A25," - ",B25)</f>
+        <v>IN - institutional</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" t="str">
+        <f>_xlfn.CONCAT(A26," - ",B26)</f>
+        <v>SC - k12 school</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" t="s">
+        <v>47</v>
+      </c>
+      <c r="C27" t="str">
+        <f>_xlfn.CONCAT(A27," - ",B27)</f>
+        <v>UN - college or university</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>43</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B28" t="s">
         <v>57</v>
       </c>
-      <c r="C26" t="str">
-        <f t="shared" si="0"/>
+      <c r="C28" t="str">
+        <f>_xlfn.CONCAT(A28," - ",B28)</f>
         <v>PA - parking lot</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+      <c r="D28" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>19</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B29" t="s">
         <v>58</v>
       </c>
-      <c r="C27" t="str">
-        <f t="shared" si="0"/>
+      <c r="C29" t="str">
+        <f>_xlfn.CONCAT(A29," - ",B29)</f>
         <v>PG - parking garage</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+      <c r="D29" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>44</v>
+      </c>
+      <c r="B30" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" t="str">
+        <f>_xlfn.CONCAT(A30," - ",B30)</f>
+        <v>LR - golf course or other low density rec use</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" t="s">
+        <v>61</v>
+      </c>
+      <c r="C31" t="str">
+        <f>_xlfn.CONCAT(A31," - ",B31)</f>
+        <v>VP - vacant permanently such as park or transport net</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>20</v>
+      </c>
+      <c r="B32" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" t="str">
+        <f>_xlfn.CONCAT(A32," - ",B32)</f>
+        <v>OT - other or unknown</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>18</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B33" t="s">
         <v>59</v>
       </c>
-      <c r="C28" t="str">
-        <f t="shared" si="0"/>
+      <c r="C33" t="str">
+        <f>_xlfn.CONCAT(A33," - ",B33)</f>
         <v>VA - vacant</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>44</v>
-      </c>
-      <c r="B29" t="s">
-        <v>60</v>
-      </c>
-      <c r="C29" t="str">
-        <f t="shared" si="0"/>
-        <v>LR - golf course or other low density rec use</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>6</v>
-      </c>
-      <c r="B30" t="s">
-        <v>61</v>
-      </c>
-      <c r="C30" t="str">
-        <f t="shared" si="0"/>
-        <v>VP - vacant permanently such as park or transport net</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>20</v>
-      </c>
-      <c r="B31" t="s">
-        <v>62</v>
-      </c>
-      <c r="C31" t="str">
-        <f t="shared" si="0"/>
-        <v>OT - other or unknown</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>45</v>
-      </c>
-      <c r="B32" t="s">
-        <v>63</v>
-      </c>
-      <c r="C32" t="str">
-        <f t="shared" si="0"/>
-        <v>IN - institutional</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>46</v>
-      </c>
-      <c r="B33" t="s">
-        <v>64</v>
-      </c>
-      <c r="C33" t="str">
-        <f t="shared" si="0"/>
-        <v>RF - retail food or drink</v>
+      <c r="D33" s="9" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D33">
+    <sortCondition ref="D2:D33"/>
+    <sortCondition ref="A2:A33"/>
+  </sortState>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>